<commit_message>
Updating SMT control board silkscreen
</commit_message>
<xml_diff>
--- a/kicad-control-board-smt/bom/kicad-control-board-smt-bom-sierra.xlsx
+++ b/kicad-control-board-smt/bom/kicad-control-board-smt-bom-sierra.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="132">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -121,19 +121,22 @@
     <t xml:space="preserve">LED</t>
   </si>
   <si>
+    <t xml:space="preserve">DNI</t>
+  </si>
+  <si>
     <t xml:space="preserve">D105,D114,D115,D111,D106,D102,D103,D107,D112,D116,D117,D113,D108,D104,D110,D101,D118,D109</t>
   </si>
   <si>
     <t xml:space="preserve">LEDs:LED_D3.0mm</t>
   </si>
   <si>
-    <t xml:space="preserve">C503B-AAS-CY0B0251-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C503B-AAS-CY0B0251</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cree</t>
+    <t xml:space="preserve">160-1940-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTL-1CHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lite-On</t>
   </si>
   <si>
     <t xml:space="preserve">Conn_01x10_Female</t>
@@ -188,9 +191,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gate Out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNI</t>
   </si>
   <si>
     <t xml:space="preserve">J104,J105,J106,J107,J108,J109</t>
@@ -430,6 +430,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -451,6 +452,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -524,17 +526,17 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="101.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="101.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="52.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="23.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="23.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.28"/>
   </cols>
@@ -679,112 +681,115 @@
       <c r="B6" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="C6" s="0" t="s">
+        <v>33</v>
+      </c>
       <c r="D6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>57</v>
@@ -1021,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>99</v>
@@ -1097,6 +1102,9 @@
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>115</v>

</xml_diff>